<commit_message>
Implemented domain and data access.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23916"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB0CFD5B-2546-41DF-81A6-6FF0162D0C8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C9BFB5-3184-43D9-8AE9-7A2AE5B2050C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>User story</t>
   </si>
@@ -67,7 +67,10 @@
     <t>Implementacija stranice za kreiranje walleta</t>
   </si>
   <si>
-    <t>Dokerizacija aplikacije i baze</t>
+    <t>Dokerizacija baze</t>
+  </si>
+  <si>
+    <t>Dokerizacija aplikacije</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -493,6 +496,9 @@
       <c r="C3">
         <v>30</v>
       </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="31.5" customHeight="1">
       <c r="B4" s="4" t="s">
@@ -501,6 +507,9 @@
       <c r="C4">
         <v>30</v>
       </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="28.5">
       <c r="B5" s="2" t="s">
@@ -555,7 +564,15 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>120</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dependency fix. Task estimation fix.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23916"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C9BFB5-3184-43D9-8AE9-7A2AE5B2050C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BD43D38-C372-4F9F-940B-BB5D3E8C5299}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>User story</t>
   </si>
@@ -46,7 +46,10 @@
     <t>Inicijalizacija projekta za domen i implementacija Wallet i Transaction klasa</t>
   </si>
   <si>
-    <t>Inicijalizacija projekta za pristup bazi podataka, osnovna podesavanja, implementacija repozitorijuma, dodavanje tabela</t>
+    <t>Inicijalizacija projekta za pristup bazi podataka, osnovna podesavanja, implementacija generickog repozitorijuma, UnitOfWorka, DbContexta</t>
+  </si>
+  <si>
+    <t>Implementacija repozitorijuma za Wallet i Tranasaction, dodavanje Tabela i konfiguracija za Wallet i Transaction</t>
   </si>
   <si>
     <t>Inicijalizacija projekta za aplikativne servise i dodavanje WalletService klase sa metodom za kreiranje Walleta</t>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,26 +508,29 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.5">
-      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.5" customHeight="1">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.5">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -532,10 +538,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="42.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -543,28 +549,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.5">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:4" ht="42.75">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5">
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
+    <row r="11" spans="1:4">
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
         <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -572,6 +578,14 @@
         <v>14</v>
       </c>
       <c r="C12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented CreateWallet method on WalletService. Added tests for WalletService.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BD43D38-C372-4F9F-940B-BB5D3E8C5299}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EAFFE0-745C-497C-BDA3-29B145926DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37845" yWindow="480" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191028"/>
 </workbook>
 </file>
 
@@ -80,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,10 +455,10 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82.5703125" customWidth="1"/>
     <col min="2" max="2" width="86.85546875" customWidth="1"/>
@@ -472,7 +466,7 @@
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25" customHeight="1">
+    <row r="1" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,12 +480,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30.75" customHeight="1">
+    <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5">
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>5</v>
@@ -503,7 +497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31.5" customHeight="1">
+    <row r="4" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -514,7 +508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31.5" customHeight="1">
+    <row r="5" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
@@ -525,39 +519,51 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.5">
+    <row r="6" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="42.75">
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.5">
+      <c r="D9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
@@ -565,7 +571,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
@@ -573,7 +579,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>14</v>
       </c>
@@ -581,7 +587,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Estimation fix and folder structure fix.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EAFFE0-745C-497C-BDA3-29B145926DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E7A1A4-19D8-4F6C-9E54-87D1B5ECF48C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37845" yWindow="480" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +549,7 @@
         <v>30</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
@@ -558,9 +558,6 @@
       </c>
       <c r="C9">
         <v>30</v>
-      </c>
-      <c r="D9">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented Controller actions and page for Deposit and updated estimations.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD99446-C9AC-4DF9-BDCB-A24E14A6ADF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D087505-FB76-48DA-B3DA-BE0D5C54C166}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37845" yWindow="480" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,6 +684,9 @@
       <c r="C19">
         <v>20</v>
       </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -691,6 +694,9 @@
       </c>
       <c r="C20">
         <v>30</v>
+      </c>
+      <c r="D20">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated estimation for system user story.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D087505-FB76-48DA-B3DA-BE0D5C54C166}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07160D2-7D87-4252-B5D8-5FDFF8171A6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37845" yWindow="480" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31590" yWindow="4620" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>User story</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Dodavanje Withdraw metode na servis za komunikaciju sa bankom</t>
+  </si>
+  <si>
+    <t>Sistem treba da limitira maksimalni iznos uplate/isplate po novcaniku na mesecnom nivou</t>
+  </si>
+  <si>
+    <t>Dodati max/min ogranicenja u appsettings.json kao njihovu proveru u PayIn/PayOut metode</t>
   </si>
 </sst>
 </file>
@@ -473,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -666,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -677,7 +683,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -688,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -697,6 +703,22 @@
       </c>
       <c r="D20">
         <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added estimation for current user story
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07160D2-7D87-4252-B5D8-5FDFF8171A6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D1F750-BF41-4A26-A83D-1E26772D860C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-31590" yWindow="4620" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>User story</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Dodati max/min ogranicenja u appsettings.json kao njihovu proveru u PayIn/PayOut metode</t>
+  </si>
+  <si>
+    <t>Kao korisnik potrebno je da mogu da prebacim novac sa naloga/novcanika na povezani bankovni racun</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,6 +724,51 @@
         <v>10</v>
       </c>
     </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed and updated task estimation. Implemented Deposit method on bank service. Implemented Withdraw method on WalletService.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D1F750-BF41-4A26-A83D-1E26772D860C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B678BF36-BFD0-41D2-A19C-71B340E723B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31590" yWindow="4620" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37410" yWindow="195" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>User story</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>Kao korisnik potrebno je da mogu da prebacim novac sa naloga/novcanika na povezani bankovni racun</t>
+  </si>
+  <si>
+    <t>Dodavanje Deposit metode na servis za komunikaciju sa bankom</t>
+  </si>
+  <si>
+    <t>Dodavanje Withdraw metode na WalletService</t>
+  </si>
+  <si>
+    <t>Implementacija testova za Withdraw</t>
+  </si>
+  <si>
+    <t>Dodavanje rute za Withdraw sredstava u WalletController</t>
+  </si>
+  <si>
+    <t>Dodavanje stranice za Withdraw sredstava u MVC aplikaciju</t>
   </si>
 </sst>
 </file>
@@ -485,7 +500,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,23 +746,29 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>10</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>25</v>
       </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>30</v>
@@ -755,7 +776,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>10</v>
@@ -763,7 +784,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>45</v>

</xml_diff>

<commit_message>
Implemented tests for withdraw method for WalletService. Implemented Withdraw page on the WebApp. Updated task estimations.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B678BF36-BFD0-41D2-A19C-71B340E723B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765CBDA8-72BF-43ED-94D6-9140401A81CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37410" yWindow="195" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +773,9 @@
       <c r="C26">
         <v>30</v>
       </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -781,6 +784,9 @@
       <c r="C27">
         <v>10</v>
       </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
@@ -788,6 +794,9 @@
       </c>
       <c r="C28">
         <v>45</v>
+      </c>
+      <c r="D28">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated task estimation for WalletTransfer user story.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765CBDA8-72BF-43ED-94D6-9140401A81CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50720B01-7C26-420E-A3B0-C44FA14F60ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37410" yWindow="195" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="3795" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>User story</t>
   </si>
@@ -113,6 +113,33 @@
   </si>
   <si>
     <t>Dodavanje stranice za Withdraw sredstava u MVC aplikaciju</t>
+  </si>
+  <si>
+    <t>Kao korisnik potrebno je da mogu da vrsim transfer novca sa svog na neki drugi novcanik u sistemu</t>
+  </si>
+  <si>
+    <t>Dodavanje Transfer metode na WalletService</t>
+  </si>
+  <si>
+    <t>Implementacija testova za Transfer</t>
+  </si>
+  <si>
+    <t>Dodavanje rute za Transfer sredstava u WalletController</t>
+  </si>
+  <si>
+    <t>Dodavanje stranice za Transfer sredstava u MVC aplikaciju</t>
+  </si>
+  <si>
+    <t>Sistem treba da racuna proviziju u slucaju transfera novca izmedju dva novcanika</t>
+  </si>
+  <si>
+    <t>Implementacija servisa za racunanje provizije</t>
+  </si>
+  <si>
+    <t>Implementacija testova za racunanje provizije</t>
+  </si>
+  <si>
+    <t>Prikaz provizije na transfer stranici</t>
   </si>
 </sst>
 </file>
@@ -497,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,6 +826,72 @@
         <v>60</v>
       </c>
     </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented tests and web app page for WalletTransfer.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50720B01-7C26-420E-A3B0-C44FA14F60ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BA8EE3C-9DE3-4667-B82C-3D23EB3FAF30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="3795" windowWidth="26385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31245" yWindow="4965" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -527,7 +528,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +839,9 @@
       <c r="C30">
         <v>20</v>
       </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -846,6 +850,9 @@
       <c r="C31">
         <v>30</v>
       </c>
+      <c r="D31">
+        <v>45</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
@@ -854,21 +861,27 @@
       <c r="C32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>37</v>
       </c>
@@ -876,7 +889,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>38</v>
       </c>
@@ -884,7 +897,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Updated task estimation for WalletBalance user story.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3656A1CD-C432-42C1-BD9B-0DE2F7FDAFED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DD02B7-D723-4C14-918C-47C57A9B45FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31245" yWindow="4965" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>User story</t>
   </si>
@@ -143,6 +143,21 @@
   </si>
   <si>
     <t>Dodavanje metode za racunanje provizije u WalletService, dodavanje provizije u Transfer metodu kao I testove za transfer</t>
+  </si>
+  <si>
+    <t>Kao korisnik potrebno je da mogu da proverim stanje na svom novcaniku u svakom trenutku</t>
+  </si>
+  <si>
+    <t>Dodavanje GetBalance metode na WalletService</t>
+  </si>
+  <si>
+    <t>Implementacija testova za GetBalance</t>
+  </si>
+  <si>
+    <t>Dodavanje rute za proveru stanja Walleta u WalletController</t>
+  </si>
+  <si>
+    <t>Dodavanje stranice za proveru stanja Walleta u MVC aplikaciju</t>
   </si>
 </sst>
 </file>
@@ -527,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +942,43 @@
         <v>90</v>
       </c>
     </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented WalletInfo method on WalletService. Implemented tests for WalletInfo. Implemented  walletInfo route and page in the web app.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DD02B7-D723-4C14-918C-47C57A9B45FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C226087-CFFE-44FB-9250-B80CC49907FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>Kao korisnik potrebno je da mogu da proverim stanje na svom novcaniku u svakom trenutku</t>
   </si>
   <si>
-    <t>Dodavanje GetBalance metode na WalletService</t>
-  </si>
-  <si>
     <t>Implementacija testova za GetBalance</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>Dodavanje stranice za proveru stanja Walleta u MVC aplikaciju</t>
+  </si>
+  <si>
+    <t>Dodavanje GetWalletInfo metode na WalletService</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,23 +949,26 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -973,7 +976,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43">
         <v>20</v>

</xml_diff>

<commit_message>
Updated estimation for Blocked wallet constraints.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE2E3D-42DB-4A9A-8965-1BC55105844E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23E5CB7-CEF0-40C8-B594-8445303E0FAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>User story</t>
   </si>
@@ -158,6 +158,18 @@
   </si>
   <si>
     <t>Dodavanje GetWalletInfo metode na WalletService</t>
+  </si>
+  <si>
+    <t>Korisniku blokiranog novcanika dozvoljene su samo operacije upita stanja I pregleda transakcija</t>
+  </si>
+  <si>
+    <t>Prosirivanje Wallet entiteta IsBlocked property-jem I Block/Unblock metodama</t>
+  </si>
+  <si>
+    <t>Dodavanje provere da li je Wallet blokiran u metode za Deposit/Withdraw/Transfer</t>
+  </si>
+  <si>
+    <t>Dodavanje testova za blokirani wallet na Deposit/Withdraw/Transfer test klase</t>
   </si>
 </sst>
 </file>
@@ -542,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,6 +1003,35 @@
         <v>45</v>
       </c>
     </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated esitmation for WalletTransactions user story.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51A4A08-D022-43CA-93A2-3B42BA59018D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD06A38E-84E8-4035-9169-9B99FE01D1A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>User story</t>
   </si>
@@ -148,15 +148,6 @@
     <t>Kao korisnik potrebno je da mogu da proverim stanje na svom novcaniku u svakom trenutku</t>
   </si>
   <si>
-    <t>Implementacija testova za GetBalance</t>
-  </si>
-  <si>
-    <t>Dodavanje rute za proveru stanja Walleta u WalletController</t>
-  </si>
-  <si>
-    <t>Dodavanje stranice za proveru stanja Walleta u MVC aplikaciju</t>
-  </si>
-  <si>
     <t>Dodavanje GetWalletInfo metode na WalletService</t>
   </si>
   <si>
@@ -170,6 +161,27 @@
   </si>
   <si>
     <t>Dodavanje testova za blokirani wallet na Deposit/Withdraw/Transfer test klase</t>
+  </si>
+  <si>
+    <t>Kao korisnik potrebno je da mogu da vidim listu svojih transakcija</t>
+  </si>
+  <si>
+    <t>Implementacija testova za GetWalletInfo</t>
+  </si>
+  <si>
+    <t>Dodavanje rute za dobijanje informacija o Walletu u WalletController</t>
+  </si>
+  <si>
+    <t>Dodavanje stranice za za dobijanje informacija o Walletu u MVC aplikaciju</t>
+  </si>
+  <si>
+    <t>Prosirivanje GetWalletInfo testova sa transakcijama</t>
+  </si>
+  <si>
+    <t>Prosirivanje ViewModela za WalletInfo transakcijama I prikaz transakcija na WalletInfo stranici</t>
+  </si>
+  <si>
+    <t>Prosirivanje GetWalletInfo sa transakcijama Walleta</t>
   </si>
 </sst>
 </file>
@@ -554,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +973,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>10</v>
@@ -972,7 +984,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C41">
         <v>20</v>
@@ -983,7 +995,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -994,7 +1006,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>30</v>
@@ -1005,12 +1017,12 @@
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -1021,7 +1033,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -1032,13 +1044,42 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C47">
         <v>10</v>
       </c>
       <c r="D47">
         <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added task estimation for ChangePassword user story. Fixed password generator.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE34E071-207C-47D1-AC27-E7E40AE6969F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE1ED47-D400-40E2-B7CB-4C74932E0873}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>User story</t>
   </si>
@@ -182,6 +182,21 @@
   </si>
   <si>
     <t>Prosirivanje GetWalletInfo sa transakcijama Walleta</t>
+  </si>
+  <si>
+    <t>Kao korisnik potrebno je da mogu da promenim svoj PASS</t>
+  </si>
+  <si>
+    <t>Dodavanje ChangePassword metode u Wallet I WalletService</t>
+  </si>
+  <si>
+    <t>Implementacija testova za ChangePassword</t>
+  </si>
+  <si>
+    <t>Dodavanje rute za ChangePassword na WalletController</t>
+  </si>
+  <si>
+    <t>Dodavanje stranice za ChangePassword u MVC aplikaciju</t>
   </si>
 </sst>
 </file>
@@ -566,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1073,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>53</v>
       </c>
@@ -1069,7 +1084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>51</v>
       </c>
@@ -1080,7 +1095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>52</v>
       </c>
@@ -1089,6 +1104,43 @@
       </c>
       <c r="D51">
         <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>57</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added estimation for admin block/unblock user story.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B60A84-0231-4AB1-988F-A15A51990BF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3CCF07-F823-4C3A-9C3F-208EE84893F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>User story</t>
   </si>
@@ -197,6 +197,24 @@
   </si>
   <si>
     <t>Dodavanje stranice za ChangePassword u MVC aplikaciju</t>
+  </si>
+  <si>
+    <t>Admin moze da blokira/odblokira odredjeni novcanik/nalog</t>
+  </si>
+  <si>
+    <t>Dodavanje admin passworda u appsetttigns</t>
+  </si>
+  <si>
+    <t>Dodavanje BlockWallet i UnblockWallet metoda u WalletService</t>
+  </si>
+  <si>
+    <t>Implementacija testova za BlockWallet I UnblockWallet</t>
+  </si>
+  <si>
+    <t>Dodavanje rute za blokiranje na WalletController</t>
+  </si>
+  <si>
+    <t>Dodavanje stranice za blokiranje u MVC aplikaciju</t>
   </si>
 </sst>
 </file>
@@ -581,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,6 +1173,51 @@
         <v>20</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Added task estimation sum.
</commit_message>
<xml_diff>
--- a/bdjakovic_Estimacija.xlsx
+++ b/bdjakovic_Estimacija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Work\WebWallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DB8E50-55C5-4D50-91E5-550D69307565}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ED60B7-3688-442B-89A5-BD25C37085D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-34470" yWindow="2700" windowWidth="29385" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,6 +1233,16 @@
         <v>25</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f>SUM(C2:C62)</f>
+        <v>1041</v>
+      </c>
+      <c r="D63">
+        <f>SUM(D2:D62)</f>
+        <v>1236</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>